<commit_message>
adding TP & Labo Starter
</commit_message>
<xml_diff>
--- a/ResultsTransformation/Map/Routes/route01.xlsx
+++ b/ResultsTransformation/Map/Routes/route01.xlsx
@@ -826,62 +826,62 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -918,62 +918,62 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1010,62 +1010,62 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1102,62 +1102,62 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -1224,62 +1224,62 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -1360,32 +1360,32 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -1452,32 +1452,32 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -1574,32 +1574,32 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -1666,32 +1666,32 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
@@ -1718,32 +1718,32 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
@@ -2037,32 +2037,32 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -2139,32 +2139,32 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
@@ -2241,32 +2241,32 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -2313,32 +2313,32 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -2365,32 +2365,32 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
@@ -2568,62 +2568,62 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
@@ -2650,62 +2650,62 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W34" t="inlineStr">
@@ -2732,62 +2732,62 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
@@ -2814,72 +2814,72 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="W36" t="inlineStr">
@@ -2956,12 +2956,12 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
@@ -3078,12 +3078,12 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -3200,12 +3200,12 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
@@ -3322,12 +3322,12 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>p</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">

</xml_diff>